<commit_message>
fix column headers and location QC
</commit_message>
<xml_diff>
--- a/bio_diversity/static/data_templates/mactaquac-collection.xlsx
+++ b/bio_diversity/static/data_templates/mactaquac-collection.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="2" r:id="rId1"/>
@@ -97,9 +97,6 @@
     <t>Time</t>
   </si>
   <si>
-    <t>Covered Bridg</t>
-  </si>
-  <si>
     <t>Destination Tank:</t>
   </si>
   <si>
@@ -110,6 +107,9 @@
   </si>
   <si>
     <t>Odell</t>
+  </si>
+  <si>
+    <t>Covered Bridge</t>
   </si>
 </sst>
 </file>
@@ -512,9 +512,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -526,13 +524,14 @@
     <col min="14" max="14" width="16.42578125" customWidth="1"/>
     <col min="15" max="15" width="16" customWidth="1"/>
     <col min="16" max="17" width="15" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.140625" customWidth="1"/>
+    <col min="18" max="18" width="16" customWidth="1"/>
     <col min="19" max="19" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="1"/>
@@ -588,7 +587,7 @@
         <v>3</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>13</v>
@@ -635,8 +634,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -655,11 +654,11 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -713,7 +712,7 @@
         <v>3</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>13</v>
@@ -757,13 +756,13 @@
         <v>19</v>
       </c>
       <c r="F3" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="K3" t="s">
         <v>20</v>
       </c>
       <c r="L3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M3" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
clean up spawning and tagging parsers
</commit_message>
<xml_diff>
--- a/bio_diversity/static/data_templates/mactaquac-collection.xlsx
+++ b/bio_diversity/static/data_templates/mactaquac-collection.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="32">
   <si>
     <t>Year</t>
   </si>
@@ -73,49 +73,49 @@
     <t>River</t>
   </si>
   <si>
-    <t>Jan</t>
-  </si>
-  <si>
     <t>PWR</t>
   </si>
   <si>
-    <t>CD, EF, GH</t>
-  </si>
-  <si>
-    <t>Fall Parr</t>
-  </si>
-  <si>
-    <t>(WS)</t>
-  </si>
-  <si>
-    <t>DC 36%, 60 Hz</t>
-  </si>
-  <si>
     <t>Time</t>
   </si>
   <si>
-    <t>LP21</t>
-  </si>
-  <si>
     <t>Group</t>
   </si>
   <si>
     <t>Odell</t>
   </si>
   <si>
-    <t>Covered Bridge</t>
-  </si>
-  <si>
     <t>Fishing Seconds</t>
   </si>
   <si>
     <t>Desitination Pond</t>
   </si>
   <si>
-    <t>LP22A</t>
-  </si>
-  <si>
     <t>Destination Pond</t>
+  </si>
+  <si>
+    <t>Apr</t>
+  </si>
+  <si>
+    <t>FP</t>
+  </si>
+  <si>
+    <t>SP3</t>
+  </si>
+  <si>
+    <t>Fundy PWR Mouth</t>
+  </si>
+  <si>
+    <t>WS</t>
+  </si>
+  <si>
+    <t>SP4</t>
+  </si>
+  <si>
+    <t>AB</t>
+  </si>
+  <si>
+    <t>CD, EF</t>
   </si>
 </sst>
 </file>
@@ -125,7 +125,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -140,6 +140,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF212529"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -197,7 +203,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -224,6 +230,14 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -506,8 +520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:U4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -555,19 +569,19 @@
         <v>2</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>16</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>12</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>4</v>
@@ -600,7 +614,7 @@
         <v>15</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="T3" s="2" t="s">
         <v>10</v>
@@ -626,8 +640,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:U5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -676,19 +690,19 @@
         <v>2</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>16</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>12</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>4</v>
@@ -721,7 +735,7 @@
         <v>15</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="T3" s="2" t="s">
         <v>10</v>
@@ -730,98 +744,99 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2020</v>
-      </c>
-      <c r="B4" t="s">
+    <row r="4" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>2021</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="1">
+        <v>5</v>
+      </c>
+      <c r="D4" s="10"/>
+      <c r="E4" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4" s="6">
-        <v>0.35416666666666669</v>
-      </c>
-      <c r="E4" t="s">
-        <v>18</v>
-      </c>
       <c r="F4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" t="s">
         <v>26</v>
       </c>
-      <c r="G4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H4" t="s">
+      <c r="I4" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="J4" s="1"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="5"/>
+      <c r="N4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="P4">
+        <v>110</v>
+      </c>
+      <c r="Q4">
+        <v>4</v>
+      </c>
+      <c r="R4" s="13">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="S4">
+        <v>350</v>
+      </c>
+      <c r="T4">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>2021</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="I4" t="s">
-        <v>27</v>
-      </c>
-      <c r="N4" t="s">
-        <v>19</v>
-      </c>
-      <c r="P4">
-        <v>18</v>
-      </c>
-      <c r="Q4">
-        <v>4.5</v>
-      </c>
-      <c r="R4" t="s">
-        <v>22</v>
-      </c>
-      <c r="S4">
-        <v>352</v>
-      </c>
-      <c r="T4">
-        <v>555</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>2020</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="C5" s="1">
+        <v>5</v>
+      </c>
+      <c r="D5" s="10"/>
+      <c r="E5" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5" s="6">
-        <v>0.59722222222222221</v>
-      </c>
-      <c r="E5" t="s">
-        <v>18</v>
-      </c>
+      <c r="F5" s="5"/>
       <c r="G5" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="H5" t="s">
-        <v>30</v>
-      </c>
-      <c r="J5">
-        <v>45.549657145988803</v>
-      </c>
-      <c r="K5">
-        <v>-65.014224771258498</v>
-      </c>
-      <c r="N5" t="s">
-        <v>19</v>
-      </c>
-      <c r="O5">
+        <v>29</v>
+      </c>
+      <c r="J5" s="11">
+        <v>45.549656159192402</v>
+      </c>
+      <c r="K5" s="1">
+        <v>-65.013694691467194</v>
+      </c>
+      <c r="L5" s="5"/>
+      <c r="N5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="P5">
+        <v>200</v>
+      </c>
+      <c r="Q5">
         <v>5</v>
       </c>
-      <c r="Q5">
-        <v>3.2</v>
-      </c>
-      <c r="R5" t="s">
-        <v>22</v>
+      <c r="R5" s="13">
+        <v>1.1000000000000001</v>
       </c>
       <c r="S5">
-        <v>800</v>
+        <v>788</v>
       </c>
       <c r="T5">
-        <v>540</v>
+        <v>500</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update collection codes to client specs
</commit_message>
<xml_diff>
--- a/bio_diversity/static/data_templates/mactaquac-collection.xlsx
+++ b/bio_diversity/static/data_templates/mactaquac-collection.xlsx
@@ -576,6 +576,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -585,8 +587,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -870,7 +870,7 @@
   <dimension ref="A2:U4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -895,29 +895,29 @@
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
       <c r="I2" s="1"/>
-      <c r="J2" s="7" t="s">
+      <c r="J2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="7"/>
-      <c r="L2" s="8" t="s">
+      <c r="K2" s="9"/>
+      <c r="L2" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="M2" s="9"/>
+      <c r="M2" s="11"/>
       <c r="N2" s="5"/>
       <c r="O2" s="5"/>
       <c r="P2" s="1"/>
     </row>
-    <row r="3" spans="1:21" s="11" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="10" t="s">
+    <row r="3" spans="1:21" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="7" t="s">
         <v>17</v>
       </c>
       <c r="E3" s="2" t="s">

</xml_diff>

<commit_message>
allow year coll to be used in collections parser
</commit_message>
<xml_diff>
--- a/bio_diversity/static/data_templates/mactaquac-collection.xlsx
+++ b/bio_diversity/static/data_templates/mactaquac-collection.xlsx
@@ -172,23 +172,12 @@
       <text>
         <r>
           <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Author:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-eg. FP</t>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Eg. 1999 BSR</t>
         </r>
       </text>
     </comment>
@@ -427,9 +416,6 @@
     <t>Temperature</t>
   </si>
   <si>
-    <t>Collection</t>
-  </si>
-  <si>
     <t># Fish Observed</t>
   </si>
   <si>
@@ -452,6 +438,9 @@
   </si>
   <si>
     <t>Destination Pond</t>
+  </si>
+  <si>
+    <t>Year Class</t>
   </si>
 </sst>
 </file>
@@ -558,7 +547,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -585,6 +574,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -870,7 +862,7 @@
   <dimension ref="A2:U4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -918,19 +910,19 @@
         <v>2</v>
       </c>
       <c r="D3" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>12</v>
+      <c r="G3" s="12" t="s">
+        <v>20</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>4</v>
@@ -951,19 +943,19 @@
         <v>3</v>
       </c>
       <c r="O3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="P3" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="Q3" s="2" t="s">
         <v>11</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="T3" s="2" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
fix bugs in parsers from movedets
</commit_message>
<xml_diff>
--- a/bio_diversity/static/data_templates/mactaquac-collection.xlsx
+++ b/bio_diversity/static/data_templates/mactaquac-collection.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA8204BB-0F5D-4AEF-93AD-E4C217AFA833}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{015A9218-2602-46C8-9DE7-58D6EAD0DA8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -286,6 +286,15 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -294,15 +303,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -587,7 +587,7 @@
   <dimension ref="A1:V3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:V2"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -612,14 +612,14 @@
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
       <c r="I1" s="1"/>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="9"/>
-      <c r="L1" s="10" t="s">
+      <c r="K1" s="12"/>
+      <c r="L1" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="11"/>
+      <c r="M1" s="14"/>
       <c r="N1" s="5"/>
       <c r="O1" s="5"/>
       <c r="P1" s="1"/>
@@ -693,71 +693,71 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:22" s="14" customFormat="1" ht="51" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+    <row r="3" spans="1:22" s="11" customFormat="1" ht="51" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="G3" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="H3" s="13" t="s">
+      <c r="H3" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="I3" s="13" t="s">
+      <c r="I3" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="J3" s="13" t="s">
+      <c r="J3" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="K3" s="13" t="s">
+      <c r="K3" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="L3" s="13" t="s">
+      <c r="L3" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="M3" s="13" t="s">
+      <c r="M3" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="N3" s="13" t="s">
+      <c r="N3" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="O3" s="13" t="s">
+      <c r="O3" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="P3" s="13" t="s">
+      <c r="P3" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="Q3" s="13" t="s">
+      <c r="Q3" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="R3" s="13" t="s">
+      <c r="R3" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="S3" s="13" t="s">
+      <c r="S3" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="T3" s="13" t="s">
+      <c r="T3" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="U3" s="13" t="s">
+      <c r="U3" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="V3" s="13" t="s">
+      <c r="V3" s="10" t="s">
         <v>38</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update container names in mactaquac parsers
</commit_message>
<xml_diff>
--- a/bio_diversity/static/data_templates/mactaquac-collection.xlsx
+++ b/bio_diversity/static/data_templates/mactaquac-collection.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{015A9218-2602-46C8-9DE7-58D6EAD0DA8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAAFB65C-FD04-49A0-9C1E-3C6C745DCD30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -103,9 +103,6 @@
     <t>Eg. Bonell. Optional</t>
   </si>
   <si>
-    <t>Optional if no salmon were brought back to facility</t>
-  </si>
-  <si>
     <t>Optional, must match with site name in database.</t>
   </si>
   <si>
@@ -146,6 +143,9 @@
   </si>
   <si>
     <t>Optional, in Volts</t>
+  </si>
+  <si>
+    <t>Optional if no salmon were brought back to facility. E.g. LP1</t>
   </si>
 </sst>
 </file>
@@ -587,7 +587,7 @@
   <dimension ref="A1:V3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -704,7 +704,7 @@
         <v>24</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E3" s="10" t="s">
         <v>25</v>
@@ -713,52 +713,52 @@
         <v>26</v>
       </c>
       <c r="G3" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="I3" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="J3" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="K3" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="L3" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="M3" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="N3" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="O3" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="P3" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q3" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="R3" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="S3" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="T3" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="U3" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="H3" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="I3" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="J3" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="K3" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="L3" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="M3" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="N3" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="O3" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="P3" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q3" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="R3" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="S3" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="T3" s="10" t="s">
+      <c r="V3" s="10" t="s">
         <v>37</v>
-      </c>
-      <c r="U3" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="V3" s="10" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>